<commit_message>
weather max acute angle opt rank
</commit_message>
<xml_diff>
--- a/weatherrankfilter_dbscan.xlsx
+++ b/weatherrankfilter_dbscan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shukl\Documents\GitHub\Daily_Weather\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620735A7-D730-4F65-9E62-0026914DB20D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19CD30C9-EEF7-496A-9A21-CED78F93874B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="6" activeTab="14" xr2:uid="{9165270A-2809-4AF8-982C-0E3B25320FC9}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="93">
   <si>
     <t>---------split 1 --------------------</t>
   </si>
@@ -639,6 +639,18 @@
   <si>
     <t>diff</t>
   </si>
+  <si>
+    <t>l1 knee error</t>
+  </si>
+  <si>
+    <t>l1 20% excision</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> knee angle opt rank</t>
+  </si>
+  <si>
+    <t>knee opt rank error</t>
+  </si>
 </sst>
 </file>
 
@@ -723,7 +735,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -823,6 +835,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.89999084444715716"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1184,7 +1202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="192">
+  <cellXfs count="213">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1456,6 +1474,35 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="18" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="18" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="18" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1534,41 +1581,65 @@
     <xf numFmtId="0" fontId="4" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="18" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="18" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="18" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="18" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="18" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="18" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="18" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="18" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1582,17 +1653,29 @@
     <xf numFmtId="0" fontId="4" fillId="17" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="17" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="17" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="17" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="17" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="17" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1606,6 +1689,18 @@
     <xf numFmtId="2" fontId="0" fillId="17" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="17" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="17" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="17" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="17" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1618,26 +1713,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -10405,26 +10482,26 @@
     <row r="2" spans="2:12" ht="15" thickBot="1">
       <c r="B2" s="49"/>
       <c r="C2" s="49"/>
-      <c r="D2" s="144" t="s">
+      <c r="D2" s="155" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="145"/>
+      <c r="E2" s="156"/>
       <c r="F2" s="50"/>
-      <c r="J2" s="144" t="s">
+      <c r="J2" s="155" t="s">
         <v>44</v>
       </c>
-      <c r="K2" s="145"/>
+      <c r="K2" s="156"/>
     </row>
     <row r="3" spans="2:12" ht="14.55" customHeight="1">
-      <c r="D3" s="146" t="s">
+      <c r="D3" s="157" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="147"/>
+      <c r="E3" s="158"/>
       <c r="F3" s="51"/>
-      <c r="J3" s="146" t="s">
+      <c r="J3" s="157" t="s">
         <v>45</v>
       </c>
-      <c r="K3" s="147"/>
+      <c r="K3" s="158"/>
     </row>
     <row r="4" spans="2:12" ht="15" thickBot="1">
       <c r="D4" s="52" t="s">
@@ -10442,7 +10519,7 @@
       </c>
     </row>
     <row r="5" spans="2:12" ht="14.55" customHeight="1">
-      <c r="B5" s="140" t="b">
+      <c r="B5" s="151" t="b">
         <v>1</v>
       </c>
       <c r="C5" s="55" t="s">
@@ -10456,10 +10533,10 @@
         <f>D14</f>
         <v>34.4</v>
       </c>
-      <c r="F5" s="142" t="s">
+      <c r="F5" s="153" t="s">
         <v>61</v>
       </c>
-      <c r="H5" s="140" t="b">
+      <c r="H5" s="151" t="b">
         <v>1</v>
       </c>
       <c r="I5" s="55" t="s">
@@ -10473,12 +10550,12 @@
         <f>D20</f>
         <v>34.9</v>
       </c>
-      <c r="L5" s="142" t="s">
+      <c r="L5" s="153" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="15" thickBot="1">
-      <c r="B6" s="141"/>
+      <c r="B6" s="152"/>
       <c r="C6" s="58" t="s">
         <v>56</v>
       </c>
@@ -10490,8 +10567,8 @@
         <f>D15</f>
         <v>124.9</v>
       </c>
-      <c r="F6" s="143"/>
-      <c r="H6" s="141"/>
+      <c r="F6" s="154"/>
+      <c r="H6" s="152"/>
       <c r="I6" s="58" t="s">
         <v>56</v>
       </c>
@@ -10503,7 +10580,7 @@
         <f>D21</f>
         <v>120.8</v>
       </c>
-      <c r="L6" s="143"/>
+      <c r="L6" s="154"/>
     </row>
     <row r="7" spans="2:12" ht="28.8">
       <c r="D7" s="73" t="s">
@@ -10795,10 +10872,10 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="133" t="s">
+      <c r="G1" s="144" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="134"/>
+      <c r="H1" s="145"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="2"/>
@@ -10820,10 +10897,10 @@
       <c r="H2" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="135" t="s">
+      <c r="I2" s="146" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="136"/>
+      <c r="J2" s="147"/>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1">
       <c r="A3" s="3">
@@ -10849,11 +10926,11 @@
         <f>SUM(D3,D6,D9,D12,D15,D18,D21,D24,D27,D30)/10</f>
         <v>23.824451400000001</v>
       </c>
-      <c r="I3" s="137">
+      <c r="I3" s="148">
         <f>(H3-G3)/H3*100</f>
         <v>3.6842103319113475</v>
       </c>
-      <c r="J3" s="138"/>
+      <c r="J3" s="149"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
@@ -11169,26 +11246,26 @@
     <row r="2" spans="2:12" ht="15" thickBot="1">
       <c r="B2" s="49"/>
       <c r="C2" s="49"/>
-      <c r="D2" s="144" t="s">
+      <c r="D2" s="155" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="145"/>
+      <c r="E2" s="156"/>
       <c r="F2" s="50"/>
-      <c r="J2" s="144" t="s">
+      <c r="J2" s="155" t="s">
         <v>44</v>
       </c>
-      <c r="K2" s="145"/>
+      <c r="K2" s="156"/>
     </row>
     <row r="3" spans="2:12" ht="14.55" customHeight="1">
-      <c r="D3" s="146" t="s">
+      <c r="D3" s="157" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="147"/>
+      <c r="E3" s="158"/>
       <c r="F3" s="51"/>
-      <c r="J3" s="146" t="s">
+      <c r="J3" s="157" t="s">
         <v>45</v>
       </c>
-      <c r="K3" s="147"/>
+      <c r="K3" s="158"/>
     </row>
     <row r="4" spans="2:12" ht="15" thickBot="1">
       <c r="D4" s="52" t="s">
@@ -11206,7 +11283,7 @@
       </c>
     </row>
     <row r="5" spans="2:12" ht="14.55" customHeight="1">
-      <c r="B5" s="140" t="b">
+      <c r="B5" s="151" t="b">
         <v>1</v>
       </c>
       <c r="C5" s="55" t="s">
@@ -11220,10 +11297,10 @@
         <f>D14</f>
         <v>34.1</v>
       </c>
-      <c r="F5" s="142" t="s">
+      <c r="F5" s="153" t="s">
         <v>71</v>
       </c>
-      <c r="H5" s="140" t="b">
+      <c r="H5" s="151" t="b">
         <v>1</v>
       </c>
       <c r="I5" s="55" t="s">
@@ -11237,12 +11314,12 @@
         <f>D20</f>
         <v>34.9</v>
       </c>
-      <c r="L5" s="142" t="s">
+      <c r="L5" s="153" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="15" thickBot="1">
-      <c r="B6" s="141"/>
+      <c r="B6" s="152"/>
       <c r="C6" s="58" t="s">
         <v>56</v>
       </c>
@@ -11254,8 +11331,8 @@
         <f>D15</f>
         <v>121.6</v>
       </c>
-      <c r="F6" s="143"/>
-      <c r="H6" s="141"/>
+      <c r="F6" s="154"/>
+      <c r="H6" s="152"/>
       <c r="I6" s="58" t="s">
         <v>56</v>
       </c>
@@ -11267,7 +11344,7 @@
         <f>D21</f>
         <v>120.8</v>
       </c>
-      <c r="L6" s="143"/>
+      <c r="L6" s="154"/>
     </row>
     <row r="7" spans="2:12" ht="28.8">
       <c r="D7" s="73" t="s">
@@ -11561,30 +11638,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1">
-      <c r="B1" s="148" t="s">
+      <c r="B1" s="159" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="149"/>
-      <c r="D1" s="150"/>
-      <c r="G1" s="148" t="s">
+      <c r="C1" s="160"/>
+      <c r="D1" s="161"/>
+      <c r="G1" s="159" t="s">
         <v>73</v>
       </c>
-      <c r="H1" s="149"/>
-      <c r="I1" s="150"/>
+      <c r="H1" s="160"/>
+      <c r="I1" s="161"/>
     </row>
     <row r="2" spans="1:14" ht="15" thickBot="1"/>
     <row r="3" spans="1:14" ht="15" thickBot="1">
       <c r="A3" s="76"/>
       <c r="B3" s="76"/>
-      <c r="C3" s="151" t="s">
+      <c r="C3" s="162" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="152"/>
+      <c r="D3" s="163"/>
       <c r="E3" s="77"/>
-      <c r="H3" s="153" t="s">
+      <c r="H3" s="164" t="s">
         <v>45</v>
       </c>
-      <c r="I3" s="154"/>
+      <c r="I3" s="165"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1">
       <c r="A4" s="76"/>
@@ -11604,7 +11681,7 @@
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="155" t="b">
+      <c r="A5" s="166" t="b">
         <v>1</v>
       </c>
       <c r="B5" s="78" t="s">
@@ -11617,7 +11694,7 @@
       <c r="I5" s="80"/>
     </row>
     <row r="6" spans="1:14" ht="15" thickBot="1">
-      <c r="A6" s="156"/>
+      <c r="A6" s="167"/>
       <c r="B6" s="81" t="s">
         <v>56</v>
       </c>
@@ -11689,10 +11766,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39BF5402-0B55-4FF7-968A-750CFC968FFA}">
-  <dimension ref="A1:S22"/>
+  <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L10"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -11701,81 +11778,95 @@
     <col min="7" max="8" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15" thickBot="1">
-      <c r="C1" s="157" t="s">
+    <row r="1" spans="1:21" ht="15" thickBot="1">
+      <c r="C1" s="186" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="187"/>
+      <c r="E1" s="186" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="187"/>
+      <c r="G1" s="188" t="s">
+        <v>84</v>
+      </c>
+      <c r="H1" s="189"/>
+      <c r="I1" s="186" t="s">
+        <v>92</v>
+      </c>
+      <c r="J1" s="187"/>
+      <c r="K1" s="186" t="s">
+        <v>91</v>
+      </c>
+      <c r="L1" s="187"/>
+      <c r="M1" s="186" t="s">
+        <v>82</v>
+      </c>
+      <c r="N1" s="187"/>
+      <c r="P1" s="168" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="158"/>
-      <c r="E1" s="157" t="s">
-        <v>83</v>
-      </c>
-      <c r="F1" s="158"/>
-      <c r="G1" s="169" t="s">
-        <v>84</v>
-      </c>
-      <c r="H1" s="170"/>
-      <c r="I1" s="157" t="s">
-        <v>86</v>
-      </c>
-      <c r="J1" s="158"/>
-      <c r="K1" s="157" t="s">
+      <c r="Q1" s="169"/>
+      <c r="R1" s="168" t="s">
         <v>82</v>
       </c>
-      <c r="L1" s="158"/>
-      <c r="N1" s="157" t="s">
-        <v>85</v>
-      </c>
-      <c r="O1" s="158"/>
-      <c r="P1" s="157" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q1" s="158"/>
-      <c r="R1" s="157" t="s">
+      <c r="S1" s="169"/>
+      <c r="T1" s="168" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="158"/>
-    </row>
-    <row r="2" spans="1:19" ht="15" thickBot="1">
+      <c r="U1" s="169"/>
+    </row>
+    <row r="2" spans="1:21" ht="15" thickBot="1">
       <c r="G2" s="106"/>
       <c r="H2" s="106"/>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" thickBot="1">
+      <c r="P2" s="134"/>
+      <c r="Q2" s="134"/>
+      <c r="R2" s="134"/>
+      <c r="S2" s="134"/>
+      <c r="T2" s="134"/>
+      <c r="U2" s="134"/>
+    </row>
+    <row r="3" spans="1:21" ht="15" customHeight="1" thickBot="1">
       <c r="A3" s="76"/>
       <c r="B3" s="76"/>
-      <c r="C3" s="185" t="s">
+      <c r="C3" s="182" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="186"/>
-      <c r="E3" s="185" t="s">
+      <c r="D3" s="183"/>
+      <c r="E3" s="182" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="186"/>
-      <c r="G3" s="171" t="s">
+      <c r="F3" s="183"/>
+      <c r="G3" s="190" t="s">
         <v>45</v>
       </c>
-      <c r="H3" s="172"/>
-      <c r="I3" s="185" t="s">
+      <c r="H3" s="191"/>
+      <c r="I3" s="182" t="s">
         <v>45</v>
       </c>
-      <c r="J3" s="186"/>
-      <c r="K3" s="153" t="s">
+      <c r="J3" s="183"/>
+      <c r="K3" s="164" t="s">
         <v>45</v>
       </c>
-      <c r="L3" s="154"/>
-      <c r="N3" s="151" t="s">
+      <c r="L3" s="165"/>
+      <c r="M3" s="164" t="s">
         <v>45</v>
       </c>
-      <c r="O3" s="152"/>
-      <c r="P3" s="153" t="s">
+      <c r="N3" s="165"/>
+      <c r="P3" s="170" t="s">
         <v>45</v>
       </c>
-      <c r="Q3" s="154"/>
-      <c r="R3" s="151" t="s">
+      <c r="Q3" s="171"/>
+      <c r="R3" s="170" t="s">
         <v>45</v>
       </c>
-      <c r="S3" s="152"/>
-    </row>
-    <row r="4" spans="1:19" ht="15" thickBot="1">
+      <c r="S3" s="177"/>
+      <c r="T3" s="170" t="s">
+        <v>45</v>
+      </c>
+      <c r="U3" s="171"/>
+    </row>
+    <row r="4" spans="1:21" ht="15" thickBot="1">
       <c r="A4" s="76"/>
       <c r="B4" s="76"/>
       <c r="C4" s="52" t="s">
@@ -11808,43 +11899,49 @@
       <c r="L4" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="N4" s="52" t="s">
+      <c r="M4" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="O4" s="53" t="s">
+      <c r="N4" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="P4" s="52" t="s">
+      <c r="P4" s="135" t="s">
         <v>55</v>
       </c>
-      <c r="Q4" s="53" t="s">
+      <c r="Q4" s="136" t="s">
         <v>56</v>
       </c>
-      <c r="R4" s="52" t="s">
+      <c r="R4" s="135" t="s">
         <v>55</v>
       </c>
-      <c r="S4" s="53" t="s">
+      <c r="S4" s="136" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="5" spans="1:19">
-      <c r="A5" s="190" t="b">
+      <c r="T4" s="135" t="s">
+        <v>55</v>
+      </c>
+      <c r="U4" s="136" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5" s="184" t="b">
         <v>1</v>
       </c>
       <c r="B5" s="78" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="187">
-        <v>0.841804</v>
-      </c>
-      <c r="D5" s="188">
-        <v>0.158196</v>
-      </c>
-      <c r="E5" s="187">
-        <v>0.72299899999999995</v>
-      </c>
-      <c r="F5" s="188">
-        <v>0.277001</v>
+      <c r="C5" s="131">
+        <v>0.87293500000000002</v>
+      </c>
+      <c r="D5" s="132">
+        <v>0.12706500000000001</v>
+      </c>
+      <c r="E5" s="131">
+        <v>0.746506</v>
+      </c>
+      <c r="F5" s="132">
+        <v>0.253494</v>
       </c>
       <c r="G5" s="123">
         <v>0.92870799999999998</v>
@@ -11852,54 +11949,60 @@
       <c r="H5" s="124">
         <v>7.1291999999999994E-2</v>
       </c>
-      <c r="I5" s="187">
-        <v>0.84879300000000002</v>
-      </c>
-      <c r="J5" s="188">
-        <v>0.15120700000000001</v>
+      <c r="I5" s="131">
+        <v>0.87865300000000002</v>
+      </c>
+      <c r="J5" s="132">
+        <v>0.121347</v>
       </c>
       <c r="K5" s="121">
-        <v>0.84434600000000004</v>
+        <v>0.87484099999999998</v>
       </c>
       <c r="L5" s="122">
-        <v>0.15565399999999999</v>
-      </c>
-      <c r="M5" s="129"/>
-      <c r="N5" s="121">
+        <v>0.12515899999999999</v>
+      </c>
+      <c r="M5" s="121">
+        <v>0.87357099999999999</v>
+      </c>
+      <c r="N5" s="122">
+        <v>0.12642900000000001</v>
+      </c>
+      <c r="O5" s="129"/>
+      <c r="P5" s="137">
         <v>0.72744599745870397</v>
       </c>
-      <c r="O5" s="122">
+      <c r="Q5" s="138">
         <v>0.27255400254129603</v>
       </c>
-      <c r="P5" s="121">
+      <c r="R5" s="137">
         <v>0.71918700000000002</v>
       </c>
-      <c r="Q5" s="122">
+      <c r="S5" s="138">
         <v>0.28081299999999998</v>
       </c>
-      <c r="R5" s="121">
+      <c r="T5" s="137">
         <v>0.72744599745870397</v>
       </c>
-      <c r="S5" s="122">
+      <c r="U5" s="138">
         <v>0.27255400254129603</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15" thickBot="1">
-      <c r="A6" s="191"/>
+    <row r="6" spans="1:21" ht="15" thickBot="1">
+      <c r="A6" s="185"/>
       <c r="B6" s="81" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="189">
-        <v>5.4455000000000003E-2</v>
+      <c r="C6" s="133">
+        <v>7.3638999999999996E-2</v>
       </c>
       <c r="D6" s="126">
-        <v>0.94554499999999997</v>
-      </c>
-      <c r="E6" s="189">
-        <v>4.5791999999999999E-2</v>
+        <v>0.92636099999999999</v>
+      </c>
+      <c r="E6" s="133">
+        <v>7.3638999999999996E-2</v>
       </c>
       <c r="F6" s="126">
-        <v>0.95420799999999995</v>
+        <v>0.92636099999999999</v>
       </c>
       <c r="G6" s="127">
         <v>0.14021</v>
@@ -11907,39 +12010,45 @@
       <c r="H6" s="128">
         <v>0.85979000000000005</v>
       </c>
-      <c r="I6" s="189">
-        <v>0.10581699999999999</v>
+      <c r="I6" s="133">
+        <v>0.10396</v>
       </c>
       <c r="J6" s="126">
-        <v>0.89418299999999995</v>
+        <v>0.89603999999999995</v>
       </c>
       <c r="K6" s="125">
-        <v>5.5073999999999998E-2</v>
+        <v>7.1781999999999999E-2</v>
       </c>
       <c r="L6" s="126">
-        <v>0.94492600000000004</v>
-      </c>
-      <c r="M6" s="129"/>
-      <c r="N6" s="125">
+        <v>0.92821799999999999</v>
+      </c>
+      <c r="M6" s="125">
+        <v>8.0446000000000004E-2</v>
+      </c>
+      <c r="N6" s="126">
+        <v>0.91955399999999998</v>
+      </c>
+      <c r="O6" s="129"/>
+      <c r="P6" s="139">
         <v>1.7945544554455399E-2</v>
       </c>
-      <c r="O6" s="126">
+      <c r="Q6" s="140">
         <v>0.98205445544554404</v>
       </c>
-      <c r="P6" s="125">
+      <c r="R6" s="139">
         <v>1.6088999999999999E-2</v>
       </c>
-      <c r="Q6" s="126">
+      <c r="S6" s="140">
         <v>0.98391099999999998</v>
       </c>
-      <c r="R6" s="125">
+      <c r="T6" s="139">
         <v>1.7945544554455399E-2</v>
       </c>
-      <c r="S6" s="126">
+      <c r="U6" s="140">
         <v>0.98205445544554404</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:21">
       <c r="C7" s="129"/>
       <c r="D7" s="129"/>
       <c r="E7" s="129"/>
@@ -11953,12 +12062,14 @@
       <c r="M7" s="129"/>
       <c r="N7" s="129"/>
       <c r="O7" s="129"/>
-      <c r="P7" s="129"/>
-      <c r="Q7" s="129"/>
-      <c r="R7" s="129"/>
-      <c r="S7" s="129"/>
-    </row>
-    <row r="8" spans="1:19" ht="15" thickBot="1">
+      <c r="P7" s="141"/>
+      <c r="Q7" s="141"/>
+      <c r="R7" s="141"/>
+      <c r="S7" s="141"/>
+      <c r="T7" s="141"/>
+      <c r="U7" s="141"/>
+    </row>
+    <row r="8" spans="1:21" ht="15" thickBot="1">
       <c r="C8" s="129"/>
       <c r="D8" s="129"/>
       <c r="E8" s="129"/>
@@ -11972,90 +12083,100 @@
       <c r="M8" s="129"/>
       <c r="N8" s="129"/>
       <c r="O8" s="129"/>
-      <c r="P8" s="129"/>
-      <c r="Q8" s="129"/>
-      <c r="R8" s="129"/>
-      <c r="S8" s="129"/>
-    </row>
-    <row r="9" spans="1:19">
+      <c r="P8" s="141"/>
+      <c r="Q8" s="141"/>
+      <c r="R8" s="141"/>
+      <c r="S8" s="141"/>
+      <c r="T8" s="141"/>
+      <c r="U8" s="141"/>
+    </row>
+    <row r="9" spans="1:21">
       <c r="A9" s="85" t="s">
         <v>74</v>
       </c>
       <c r="B9" s="86"/>
-      <c r="C9" s="159">
-        <v>0.94554499999999997</v>
-      </c>
-      <c r="D9" s="160"/>
-      <c r="E9" s="159">
-        <v>0.95420799999999995</v>
-      </c>
-      <c r="F9" s="160"/>
-      <c r="G9" s="177">
+      <c r="C9" s="192">
+        <v>0.92636099999999999</v>
+      </c>
+      <c r="D9" s="193"/>
+      <c r="E9" s="192">
+        <v>0.92636099999999999</v>
+      </c>
+      <c r="F9" s="193"/>
+      <c r="G9" s="200">
         <v>0.85979000000000005</v>
       </c>
-      <c r="H9" s="178"/>
-      <c r="I9" s="159">
-        <v>0.89418299999999995</v>
-      </c>
-      <c r="J9" s="160"/>
-      <c r="K9" s="164">
-        <v>0.94492600000000004</v>
-      </c>
-      <c r="L9" s="165"/>
-      <c r="M9" s="129"/>
-      <c r="N9" s="159">
+      <c r="H9" s="201"/>
+      <c r="I9" s="192">
+        <v>0.89603999999999995</v>
+      </c>
+      <c r="J9" s="193"/>
+      <c r="K9" s="194">
+        <v>0.92821799999999999</v>
+      </c>
+      <c r="L9" s="195"/>
+      <c r="M9" s="194">
+        <v>0.91955399999999998</v>
+      </c>
+      <c r="N9" s="195"/>
+      <c r="O9" s="129"/>
+      <c r="P9" s="172">
         <v>0.98205445544554404</v>
       </c>
-      <c r="O9" s="160"/>
-      <c r="P9" s="164">
+      <c r="Q9" s="173"/>
+      <c r="R9" s="178">
         <v>0.98391099999999998</v>
       </c>
-      <c r="Q9" s="165"/>
-      <c r="R9" s="159">
+      <c r="S9" s="179"/>
+      <c r="T9" s="172">
         <v>0.98205445544554404</v>
       </c>
-      <c r="S9" s="160"/>
-    </row>
-    <row r="10" spans="1:19" ht="15" thickBot="1">
+      <c r="U9" s="173"/>
+    </row>
+    <row r="10" spans="1:21" ht="15" thickBot="1">
       <c r="A10" s="88" t="s">
         <v>75</v>
       </c>
       <c r="B10" s="89"/>
-      <c r="C10" s="161">
-        <v>0.158196</v>
-      </c>
-      <c r="D10" s="162"/>
-      <c r="E10" s="161">
-        <v>0.277001</v>
-      </c>
-      <c r="F10" s="162"/>
-      <c r="G10" s="179">
+      <c r="C10" s="196">
+        <v>0.12706500000000001</v>
+      </c>
+      <c r="D10" s="197"/>
+      <c r="E10" s="196">
+        <v>0.253494</v>
+      </c>
+      <c r="F10" s="197"/>
+      <c r="G10" s="202">
         <v>7.1291999999999994E-2</v>
       </c>
-      <c r="H10" s="180"/>
-      <c r="I10" s="161">
-        <v>0.15120700000000001</v>
-      </c>
-      <c r="J10" s="162"/>
-      <c r="K10" s="166">
-        <v>0.15565399999999999</v>
-      </c>
-      <c r="L10" s="167"/>
-      <c r="M10" s="129"/>
-      <c r="N10" s="161">
+      <c r="H10" s="203"/>
+      <c r="I10" s="196">
+        <v>0.121347</v>
+      </c>
+      <c r="J10" s="197"/>
+      <c r="K10" s="198">
+        <v>0.12515899999999999</v>
+      </c>
+      <c r="L10" s="199"/>
+      <c r="M10" s="198">
+        <v>0.12642900000000001</v>
+      </c>
+      <c r="N10" s="199"/>
+      <c r="O10" s="129"/>
+      <c r="P10" s="174">
         <v>0.27255400254129603</v>
       </c>
-      <c r="O10" s="162"/>
-      <c r="P10" s="166">
+      <c r="Q10" s="175"/>
+      <c r="R10" s="180">
         <v>0.28081299999999998</v>
       </c>
-      <c r="Q10" s="167"/>
-      <c r="R10" s="161">
+      <c r="S10" s="181"/>
+      <c r="T10" s="174">
         <v>0.27255400254129603</v>
       </c>
-      <c r="S10" s="162"/>
-    </row>
-    <row r="11" spans="1:19">
+      <c r="U10" s="175"/>
+    </row>
+    <row r="11" spans="1:21">
       <c r="C11" s="97"/>
       <c r="D11" s="97"/>
       <c r="E11" s="97"/>
@@ -12066,8 +12187,10 @@
       <c r="J11" s="97"/>
       <c r="K11" s="97"/>
       <c r="L11" s="97"/>
-    </row>
-    <row r="12" spans="1:19" ht="15" thickBot="1">
+      <c r="M11" s="97"/>
+      <c r="N11" s="97"/>
+    </row>
+    <row r="12" spans="1:21" ht="15" thickBot="1">
       <c r="C12" s="97"/>
       <c r="D12" s="97"/>
       <c r="E12" s="97"/>
@@ -12078,96 +12201,107 @@
       <c r="J12" s="97"/>
       <c r="K12" s="97"/>
       <c r="L12" s="105"/>
-    </row>
-    <row r="13" spans="1:19" ht="15" thickBot="1">
+      <c r="M12" s="97"/>
+      <c r="N12" s="105"/>
+    </row>
+    <row r="13" spans="1:21" ht="15" thickBot="1">
       <c r="A13" s="119" t="s">
         <v>76</v>
       </c>
       <c r="B13" s="120"/>
-      <c r="C13" s="173">
+      <c r="C13" s="204">
         <v>0.10815</v>
       </c>
-      <c r="D13" s="174"/>
-      <c r="E13" s="173">
+      <c r="D13" s="205"/>
+      <c r="E13" s="204">
         <v>0.15767999999999999</v>
       </c>
-      <c r="F13" s="174"/>
-      <c r="G13" s="175">
+      <c r="F13" s="205"/>
+      <c r="G13" s="206">
         <v>0.10627</v>
       </c>
-      <c r="H13" s="176"/>
-      <c r="I13" s="173">
+      <c r="H13" s="207"/>
+      <c r="I13" s="204">
         <v>0.121944</v>
       </c>
-      <c r="J13" s="174"/>
-      <c r="K13" s="175">
+      <c r="J13" s="205"/>
+      <c r="K13" s="206">
         <v>0.107837</v>
       </c>
-      <c r="L13" s="176"/>
-      <c r="N13" s="163" t="s">
+      <c r="L13" s="207"/>
+      <c r="M13" s="206">
+        <v>0.107837</v>
+      </c>
+      <c r="N13" s="207"/>
+      <c r="P13" s="176" t="s">
         <v>88</v>
       </c>
-      <c r="O13" s="163"/>
-      <c r="P13" s="163"/>
-      <c r="Q13" s="163"/>
-      <c r="R13" s="163"/>
-      <c r="S13" s="163"/>
-    </row>
-    <row r="14" spans="1:19">
+      <c r="Q13" s="176"/>
+      <c r="R13" s="176"/>
+      <c r="S13" s="176"/>
+      <c r="T13" s="176"/>
+      <c r="U13" s="176"/>
+    </row>
+    <row r="14" spans="1:21">
       <c r="A14" s="92"/>
     </row>
-    <row r="20" spans="14:15" ht="15" thickBot="1"/>
-    <row r="21" spans="14:15">
-      <c r="N21" s="164"/>
-      <c r="O21" s="165"/>
-    </row>
-    <row r="22" spans="14:15" ht="15" thickBot="1">
-      <c r="N22" s="166"/>
-      <c r="O22" s="167"/>
+    <row r="20" spans="16:17" ht="15" thickBot="1"/>
+    <row r="21" spans="16:17">
+      <c r="P21" s="194"/>
+      <c r="Q21" s="195"/>
+    </row>
+    <row r="22" spans="16:17" ht="15" thickBot="1">
+      <c r="P22" s="198"/>
+      <c r="Q22" s="199"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="N22:O22"/>
+  <mergeCells count="46">
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="P22:Q22"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="E13:F13"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
     <mergeCell ref="K13:L13"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="E9:F9"/>
-    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="E10:F10"/>
-    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="K10:L10"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
-    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="T9:U9"/>
+    <mergeCell ref="T10:U10"/>
+    <mergeCell ref="P13:U13"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="P10:Q10"/>
     <mergeCell ref="R1:S1"/>
     <mergeCell ref="R3:S3"/>
     <mergeCell ref="R9:S9"/>
     <mergeCell ref="R10:S10"/>
-    <mergeCell ref="N13:S13"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="P10:Q10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -12185,26 +12319,26 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:15" ht="15" thickBot="1">
-      <c r="C1" s="157" t="s">
+      <c r="C1" s="186" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="158"/>
-      <c r="E1" s="157" t="s">
+      <c r="D1" s="187"/>
+      <c r="E1" s="186" t="s">
         <v>83</v>
       </c>
-      <c r="F1" s="158"/>
-      <c r="G1" s="169" t="s">
+      <c r="F1" s="187"/>
+      <c r="G1" s="188" t="s">
         <v>84</v>
       </c>
-      <c r="H1" s="170"/>
-      <c r="I1" s="157" t="s">
+      <c r="H1" s="189"/>
+      <c r="I1" s="186" t="s">
         <v>82</v>
       </c>
-      <c r="J1" s="158"/>
-      <c r="N1" s="157" t="s">
+      <c r="J1" s="187"/>
+      <c r="N1" s="186" t="s">
         <v>86</v>
       </c>
-      <c r="O1" s="158"/>
+      <c r="O1" s="187"/>
     </row>
     <row r="2" spans="1:15" ht="15" thickBot="1">
       <c r="G2" s="106"/>
@@ -12215,26 +12349,26 @@
     <row r="3" spans="1:15" ht="15" thickBot="1">
       <c r="A3" s="76"/>
       <c r="B3" s="76"/>
-      <c r="C3" s="151" t="s">
+      <c r="C3" s="162" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="152"/>
-      <c r="E3" s="151" t="s">
+      <c r="D3" s="163"/>
+      <c r="E3" s="162" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="152"/>
-      <c r="G3" s="171" t="s">
+      <c r="F3" s="163"/>
+      <c r="G3" s="190" t="s">
         <v>45</v>
       </c>
-      <c r="H3" s="172"/>
-      <c r="I3" s="153" t="s">
+      <c r="H3" s="191"/>
+      <c r="I3" s="164" t="s">
         <v>45</v>
       </c>
-      <c r="J3" s="154"/>
-      <c r="N3" s="153" t="s">
+      <c r="J3" s="165"/>
+      <c r="N3" s="164" t="s">
         <v>45</v>
       </c>
-      <c r="O3" s="168"/>
+      <c r="O3" s="212"/>
     </row>
     <row r="4" spans="1:15" ht="15" thickBot="1">
       <c r="A4" s="76"/>
@@ -12271,7 +12405,7 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15" thickBot="1">
-      <c r="A5" s="155" t="b">
+      <c r="A5" s="166" t="b">
         <v>1</v>
       </c>
       <c r="B5" s="78" t="s">
@@ -12309,7 +12443,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15" thickBot="1">
-      <c r="A6" s="156"/>
+      <c r="A6" s="167"/>
       <c r="B6" s="81" t="s">
         <v>56</v>
       </c>
@@ -12373,52 +12507,52 @@
         <v>74</v>
       </c>
       <c r="B9" s="86"/>
-      <c r="C9" s="159">
+      <c r="C9" s="192">
         <v>0.88923300000000005</v>
       </c>
-      <c r="D9" s="160"/>
-      <c r="E9" s="159">
+      <c r="D9" s="193"/>
+      <c r="E9" s="192">
         <v>0.90965300000000004</v>
       </c>
-      <c r="F9" s="160"/>
-      <c r="G9" s="177">
+      <c r="F9" s="193"/>
+      <c r="G9" s="200">
         <v>0.85979000000000005</v>
       </c>
-      <c r="H9" s="178"/>
-      <c r="I9" s="164">
+      <c r="H9" s="201"/>
+      <c r="I9" s="194">
         <v>0.88737600000000005</v>
       </c>
-      <c r="J9" s="165"/>
-      <c r="N9" s="183">
+      <c r="J9" s="195"/>
+      <c r="N9" s="210">
         <v>0.86509899999999995</v>
       </c>
-      <c r="O9" s="184"/>
+      <c r="O9" s="211"/>
     </row>
     <row r="10" spans="1:15" ht="15" thickBot="1">
       <c r="A10" s="88" t="s">
         <v>75</v>
       </c>
       <c r="B10" s="89"/>
-      <c r="C10" s="161">
+      <c r="C10" s="196">
         <v>0.10419299999999999</v>
       </c>
-      <c r="D10" s="162"/>
-      <c r="E10" s="161">
+      <c r="D10" s="197"/>
+      <c r="E10" s="196">
         <v>0.22045699999999999</v>
       </c>
-      <c r="F10" s="162"/>
-      <c r="G10" s="179">
+      <c r="F10" s="197"/>
+      <c r="G10" s="202">
         <v>7.1291999999999994E-2</v>
       </c>
-      <c r="H10" s="180"/>
-      <c r="I10" s="166">
+      <c r="H10" s="203"/>
+      <c r="I10" s="198">
         <v>0.102922</v>
       </c>
-      <c r="J10" s="167"/>
-      <c r="N10" s="181">
+      <c r="J10" s="199"/>
+      <c r="N10" s="208">
         <v>0.115629</v>
       </c>
-      <c r="O10" s="182"/>
+      <c r="O10" s="209"/>
     </row>
     <row r="11" spans="1:15">
       <c r="C11" s="97"/>
@@ -25330,10 +25464,10 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="131" t="s">
+      <c r="G1" s="142" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="132"/>
+      <c r="H1" s="143"/>
       <c r="J1" s="14"/>
     </row>
     <row r="2" spans="1:16">
@@ -25781,10 +25915,10 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="131" t="s">
+      <c r="G1" s="142" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="132"/>
+      <c r="H1" s="143"/>
       <c r="J1" s="14"/>
     </row>
     <row r="2" spans="1:16">
@@ -26234,10 +26368,10 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="133" t="s">
+      <c r="G1" s="144" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="134"/>
+      <c r="H1" s="145"/>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="2"/>
@@ -26259,10 +26393,10 @@
       <c r="H2" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="135" t="s">
+      <c r="I2" s="146" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="136"/>
+      <c r="J2" s="147"/>
     </row>
     <row r="3" spans="1:16" ht="15" thickBot="1">
       <c r="A3" s="3">
@@ -26288,11 +26422,11 @@
         <f>SUM(D3,D6,D9,D12,D15,D18,D21,D24,D27,D30)/10</f>
         <v>23.824451400000001</v>
       </c>
-      <c r="I3" s="137">
+      <c r="I3" s="148">
         <f>(H3-G3)/H3*100</f>
         <v>8.5526317722472331</v>
       </c>
-      <c r="J3" s="138"/>
+      <c r="J3" s="149"/>
     </row>
     <row r="4" spans="1:16" ht="15" thickBot="1">
       <c r="A4" s="1" t="s">
@@ -26696,10 +26830,10 @@
       <c r="C1" s="46"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="B2" s="139" t="s">
+      <c r="B2" s="150" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="139"/>
+      <c r="C2" s="150"/>
       <c r="D2" s="44"/>
     </row>
     <row r="3" spans="1:6">
@@ -26731,8 +26865,8 @@
       <c r="F8" s="46"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="D9" s="139"/>
-      <c r="E9" s="139"/>
+      <c r="D9" s="150"/>
+      <c r="E9" s="150"/>
       <c r="F9" s="44"/>
     </row>
     <row r="10" spans="1:6">

</xml_diff>